<commit_message>
Update, delete e select + Mudança de chave estrangeira
</commit_message>
<xml_diff>
--- a/Dicionário de dados Creche.xlsx
+++ b/Dicionário de dados Creche.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="86">
   <si>
     <t>Tabela</t>
   </si>
@@ -252,15 +252,9 @@
     <t>Not Null; PK; FK(Creche)</t>
   </si>
   <si>
-    <t>Código do funcionário da creche</t>
-  </si>
-  <si>
     <t>Not Null; FK(Aluno)</t>
   </si>
   <si>
-    <t>Not Null; FK(Funcionario)</t>
-  </si>
-  <si>
     <t>sexo</t>
   </si>
   <si>
@@ -277,6 +271,9 @@
   </si>
   <si>
     <t>varchar(80)</t>
+  </si>
+  <si>
+    <t>Not Null; FK</t>
   </si>
 </sst>
 </file>
@@ -548,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -577,6 +574,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -880,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,7 +961,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
@@ -1138,7 +1136,7 @@
       <c r="A25" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -1201,22 +1199,14 @@
         <v>52</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>80</v>
-      </c>
+      <c r="A30" s="9"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
@@ -1309,13 +1299,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>23</v>
@@ -1368,7 +1358,7 @@
         <v>49</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>57</v>
@@ -1465,10 +1455,18 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="18"/>
-      <c r="B54" s="19"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="20"/>
+      <c r="A54" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D54" s="20" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1611,7 +1609,7 @@
         <v>17</v>
       </c>
       <c r="D70" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Atualizando as entidades reponsavel e funcionario e a documentação do projeto
</commit_message>
<xml_diff>
--- a/Dicionário de dados Creche.xlsx
+++ b/Dicionário de dados Creche.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinicius\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81AA636-BCED-4F82-9361-A7060704A48D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="272"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="92">
   <si>
     <t>Tabela</t>
   </si>
@@ -126,9 +120,6 @@
     <t>varchar(14)</t>
   </si>
   <si>
-    <t>int(8)</t>
-  </si>
-  <si>
     <t>matricula</t>
   </si>
   <si>
@@ -280,12 +271,33 @@
   </si>
   <si>
     <t>Not Null; FK</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Status que define se a creche tem vagas disponíveis ou não</t>
+  </si>
+  <si>
+    <t>varchar(10)</t>
+  </si>
+  <si>
+    <t>senha</t>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+  </si>
+  <si>
+    <t>Senha do responsável</t>
+  </si>
+  <si>
+    <t>Senha do funcionário</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -336,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -346,6 +358,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,7 +379,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -404,9 +417,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -439,26 +452,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -491,26 +487,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -683,11 +662,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D68"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,12 +742,12 @@
         <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
@@ -781,28 +760,28 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="A8" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>23</v>
@@ -810,13 +789,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>23</v>
@@ -824,129 +803,129 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>25</v>
+      <c r="A14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>12</v>
+        <v>29</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>23</v>
@@ -954,13 +933,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>23</v>
@@ -968,13 +947,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>23</v>
@@ -982,13 +961,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>23</v>
@@ -996,143 +975,137 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
+      <c r="C26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="D33" s="1" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>23</v>
@@ -1140,13 +1113,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>23</v>
@@ -1154,99 +1127,99 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D38" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
+      <c r="A39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
+      <c r="A40" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
+      <c r="A42" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>23</v>
@@ -1254,43 +1227,59 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
+      <c r="A48" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
+      <c r="A49" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
@@ -1300,71 +1289,71 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C52" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D54" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
@@ -1374,71 +1363,71 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C59" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
+      <c r="B63" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>75</v>
+        <v>7</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
@@ -1448,44 +1437,70 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C66" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+      <c r="D70" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>77</v>
+      <c r="C71" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1501,7 +1516,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0"/>
@@ -1513,7 +1528,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>